<commit_message>
fix minor conflict between tags.
</commit_message>
<xml_diff>
--- a/doc/mmlcare.xlsx
+++ b/doc/mmlcare.xlsx
@@ -592,17 +592,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>mmlVs:observer</t>
-  </si>
-  <si>
-    <t>mmlVs:obsCode</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>mmlVs:obsCodeId</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>#REQUIRED</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -652,6 +641,18 @@
   </si>
   <si>
     <t>1.1.5</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>mmlFs:observer</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>mmlFs:obsCode</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>mmlFs:obsCodeId</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1072,8 +1073,8 @@
   </sheetPr>
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1114,7 +1115,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1131,7 +1132,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -1163,7 +1164,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1177,7 +1178,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>7</v>
@@ -1280,7 +1281,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">
@@ -1295,7 +1296,7 @@
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>5</v>
@@ -1311,7 +1312,7 @@
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>5</v>
@@ -1323,7 +1324,7 @@
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>15</v>
@@ -1331,7 +1332,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -1375,7 +1376,7 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>76</v>
@@ -1395,7 +1396,7 @@
         <v>16</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F25" s="2"/>
     </row>
@@ -1410,13 +1411,13 @@
         <v>5</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>80</v>
@@ -1425,13 +1426,13 @@
         <v>41</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>81</v>
@@ -1440,13 +1441,13 @@
         <v>58</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>82</v>
@@ -1455,13 +1456,13 @@
         <v>58</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>79</v>
@@ -1470,7 +1471,7 @@
         <v>5</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F30" s="2"/>
     </row>
@@ -1484,7 +1485,7 @@
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F31" s="2"/>
       <c r="H31" s="8" t="s">
@@ -1499,10 +1500,10 @@
         <v>84</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>76</v>
@@ -1522,7 +1523,7 @@
         <v>16</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F33" s="2"/>
       <c r="H33" s="8" t="s">
@@ -1540,7 +1541,7 @@
         <v>5</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F34" s="2"/>
       <c r="H34" s="8" t="s">
@@ -1558,7 +1559,7 @@
         <v>5</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F35" s="2"/>
       <c r="H35" s="8" t="s">
@@ -1574,7 +1575,7 @@
         <v>5</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F36" s="2"/>
       <c r="H36" s="8" t="s">
@@ -1592,7 +1593,7 @@
         <v>5</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F37" s="2"/>
       <c r="H37" s="2" t="s">
@@ -1610,7 +1611,7 @@
         <v>59</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1624,7 +1625,7 @@
         <v>60</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1651,7 +1652,7 @@
         <v>16</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F41" s="2"/>
     </row>
@@ -1666,7 +1667,7 @@
         <v>17</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F42" s="2"/>
     </row>
@@ -1681,7 +1682,7 @@
         <v>17</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F43" s="2"/>
     </row>
@@ -1696,12 +1697,12 @@
         <v>5</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>69</v>
@@ -1763,7 +1764,7 @@
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
Fixed inconsistency and redunduncy.
</commit_message>
<xml_diff>
--- a/doc/mmlcare.xlsx
+++ b/doc/mmlcare.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="15000" windowHeight="7830"/>
+    <workbookView xWindow="360" yWindow="405" windowWidth="15000" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$78</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$69</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="136">
   <si>
     <t>Elements</t>
   </si>
@@ -436,30 +436,12 @@
     <t>mmlFs:wardCodeId</t>
   </si>
   <si>
-    <t>mmlFs:repMemo</t>
-  </si>
-  <si>
-    <t>mmlFs:repCodeName</t>
-  </si>
-  <si>
-    <t>mmlFs:repCode</t>
-  </si>
-  <si>
-    <t>mmlFs:repCodeId</t>
-  </si>
-  <si>
-    <t>mmlFs:repMemoF</t>
-  </si>
-  <si>
     <t>mmlFs:intake</t>
   </si>
   <si>
     <t>mmlFs:intakeType</t>
   </si>
   <si>
-    <t>mmlFs000?</t>
-  </si>
-  <si>
     <t>mmlFs:intakeVolume</t>
   </si>
   <si>
@@ -517,9 +499,6 @@
     <t>mmlFs:bofPeriodEnd</t>
   </si>
   <si>
-    <t>mmlFs:bofMemo</t>
-  </si>
-  <si>
     <t>mmlFs:facility</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -544,58 +523,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>1.5.1</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1.5.2</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1.5.3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1.5.4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1.5.5</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1.5.6</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1.5.7</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1.5.8</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1.5.8.1</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1.5.8.2</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1.5.8.3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1.5.8.4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>#REQUIRED</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>#IMPLIED</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -608,7 +535,87 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>#IMPLIED</t>
+    <t>1.4.6</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.4.7</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>mmlFs:FlowSheetModule</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.1.5</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>mmlFs:observer</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>mmlFs:obsCode</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>mmlFs:obsCodeId</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.3.1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.3.2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.3.3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.3.4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.3.5</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>mmlFs01</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.3.6</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.3.7</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>mmlFs02</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>mmlFs03</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>mmlFs04</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -620,39 +627,59 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>1.4.6</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1.4.7</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>mmlFs:FlowSheetModule</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1.6</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1.7</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1.1.5</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>mmlFs:observer</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>mmlFs:obsCode</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>mmlFs:obsCodeId</t>
+    <t>1.4.8</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.5</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>mmlFs:boMemo</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>mmlFs:fsMemo</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.4.9</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.4.9.1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.4.9.2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.4.9.3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.4.10</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>?</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1071,10 +1098,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1115,7 +1142,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1127,12 +1154,12 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -1140,7 +1167,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
@@ -1164,7 +1191,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1178,7 +1205,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>7</v>
@@ -1281,7 +1308,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">
@@ -1296,7 +1323,7 @@
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>5</v>
@@ -1312,7 +1339,7 @@
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>5</v>
@@ -1322,594 +1349,531 @@
       </c>
       <c r="F15" s="11"/>
     </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="H18" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E21" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F21" s="2"/>
+        <v>131</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="4">
-        <v>1.3</v>
+      <c r="A22" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="E22" s="2" t="s">
-        <v>14</v>
+        <v>131</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="4">
-        <v>1.4</v>
+      <c r="A23" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="E23" s="2" t="s">
-        <v>14</v>
+        <v>131</v>
       </c>
       <c r="F23" s="2"/>
-      <c r="H23" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="E24" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>21</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="H26" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="D27" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F27" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="F28" s="2"/>
+      <c r="H28" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F29" s="2"/>
+        <v>131</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="F30" s="2"/>
+      <c r="H30" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="4">
-        <v>1.5</v>
+      <c r="A31" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E31" s="2" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="F31" s="2"/>
       <c r="H31" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="H32" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B33" s="2" t="s">
+      <c r="D33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F33" s="2"/>
-      <c r="H33" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="E36" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F34" s="2"/>
-      <c r="H34" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="E39" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F35" s="2"/>
-      <c r="H35" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="4"/>
-      <c r="B36" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F36" s="2"/>
-      <c r="H36" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F37" s="2"/>
-      <c r="H37" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
       <c r="E40" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="4"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="4"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="4"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A46" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A47" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A48" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A49" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A50" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A51" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A52" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A53" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A55" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A55" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A56" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A57" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A58" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A59" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A60" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A61" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A62" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A64" s="9" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A65" s="5" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A66" s="5" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A67" s="5" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A68" s="5" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A69" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A70" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A71" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A73" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A74" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A75" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A76" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A77" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A78" s="5" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>